<commit_message>
update cashflows breakdown results
</commit_message>
<xml_diff>
--- a/use_cases/LWR_FT_2023/run/results.xlsx
+++ b/use_cases/LWR_FT_2023/run/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWR_FT_2023/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0579A91-2058-934F-A42D-D073C10A0486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4CA027-0D71-DE45-848A-07894F59EC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17000" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17000" activeTab="1" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,96 @@
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">cashflow_comparison!$A$17</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">cashflow_comparison!$A$18</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">cashflow_comparison!$B$21:$N$21</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">cashflow_comparison!$A$17</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">cashflow_comparison!$A$18</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">cashflow_comparison!$A$19</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">cashflow_comparison!$A$20</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">cashflow_comparison!$A$21</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">cashflow_comparison!$B$16:$N$16</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">cashflow_comparison!$B$17:$N$17</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">cashflow_comparison!$B$18:$N$18</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">cashflow_comparison!$B$19:$N$19</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">cashflow_comparison!$A$19</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">cashflow_comparison!$B$20:$N$20</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">cashflow_comparison!$B$21:$N$21</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">cashflow_comparison!$A$17</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">cashflow_comparison!$A$18</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">cashflow_comparison!$A$19</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">cashflow_comparison!$A$20</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">cashflow_comparison!$A$21</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">cashflow_comparison!$B$16:$N$16</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">cashflow_comparison!$B$17:$N$17</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">cashflow_comparison!$B$18:$N$18</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">cashflow_comparison!$A$20</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">cashflow_comparison!$B$19:$N$19</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">cashflow_comparison!$B$20:$N$20</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">cashflow_comparison!$B$21:$N$21</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">cashflow_comparison!$A$17</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">cashflow_comparison!$A$18</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">cashflow_comparison!$A$19</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">cashflow_comparison!$A$20</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">cashflow_comparison!$A$21</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">cashflow_comparison!$B$16:$N$16</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">cashflow_comparison!$B$17:$N$17</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">cashflow_comparison!$A$21</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">cashflow_comparison!$B$18:$N$18</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">cashflow_comparison!$B$19:$N$19</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">cashflow_comparison!$B$20:$N$20</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">cashflow_comparison!$B$21:$N$21</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">cashflow_comparison!$A$17</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">cashflow_comparison!$A$18</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">cashflow_comparison!$A$19</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">cashflow_comparison!$A$20</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">cashflow_comparison!$A$21</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">cashflow_comparison!$B$16:$N$16</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">cashflow_comparison!$B$16:$N$16</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">cashflow_comparison!$B$17:$N$17</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">cashflow_comparison!$B$18:$N$18</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">cashflow_comparison!$B$19:$N$19</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">cashflow_comparison!$B$20:$N$20</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">cashflow_comparison!$B$21:$N$21</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">cashflow_comparison!$A$10</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">cashflow_comparison!$A$11</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">cashflow_comparison!$A$12</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">cashflow_comparison!$A$13</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">cashflow_comparison!$A$14</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">cashflow_comparison!$B$17:$N$17</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">cashflow_comparison!$B$10:$N$10</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">cashflow_comparison!$B$11:$N$11</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">cashflow_comparison!$B$12:$N$12</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">cashflow_comparison!$B$13:$N$13</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">cashflow_comparison!$B$14:$N$14</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">cashflow_comparison!$B$9:$N$9</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">cashflow_comparison!$A$10</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">cashflow_comparison!$A$11</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">cashflow_comparison!$A$12</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">cashflow_comparison!$A$13</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">cashflow_comparison!$B$18:$N$18</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">cashflow_comparison!$A$14</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">cashflow_comparison!$B$10:$N$10</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">cashflow_comparison!$B$11:$N$11</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">cashflow_comparison!$B$12:$N$12</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">cashflow_comparison!$B$13:$N$13</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">cashflow_comparison!$B$14:$N$14</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">cashflow_comparison!$B$9:$N$9</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">cashflow_comparison!$B$19:$N$19</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">cashflow_comparison!$B$20:$N$20</definedName>
+    <definedName name="_xlchart.v2.77" hidden="1">cashflow_comparison!$A$10</definedName>
+    <definedName name="_xlchart.v2.78" hidden="1">cashflow_comparison!$A$11</definedName>
+    <definedName name="_xlchart.v2.79" hidden="1">cashflow_comparison!$A$12</definedName>
+    <definedName name="_xlchart.v2.80" hidden="1">cashflow_comparison!$A$13</definedName>
+    <definedName name="_xlchart.v2.81" hidden="1">cashflow_comparison!$A$14</definedName>
+    <definedName name="_xlchart.v2.82" hidden="1">cashflow_comparison!$B$10:$N$10</definedName>
+    <definedName name="_xlchart.v2.83" hidden="1">cashflow_comparison!$B$11:$N$11</definedName>
+    <definedName name="_xlchart.v2.84" hidden="1">cashflow_comparison!$B$12:$N$12</definedName>
+    <definedName name="_xlchart.v2.85" hidden="1">cashflow_comparison!$B$13:$N$13</definedName>
+    <definedName name="_xlchart.v2.86" hidden="1">cashflow_comparison!$B$14:$N$14</definedName>
+    <definedName name="_xlchart.v2.87" hidden="1">cashflow_comparison!$B$9:$N$9</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1037,895 +1127,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]Sheet1!$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Braidwood</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$B$14:$M$14</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>HTSE CAPEX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>HTSE OM</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Cap Market</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>FT CAPEX</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FT OM</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>CO2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>H2 PTC</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Electricity sales</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Naphta</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Diesel</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Jet fuel</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Storage CAPEX</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]Sheet1!$B$15:$M$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>-659880291.82986307</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-500016329.72802901</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-283687374.01916456</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-259751536.196316</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-230809403.49076161</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-772932308.83213401</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4780292061.4843102</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>181380.53936527201</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>289357020.33652401</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>332766855.70381898</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>712866784.515607</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-5000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-90EA-8046-8EBE-135350765211}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]Sheet1!$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Cooper</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$B$14:$M$14</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>HTSE CAPEX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>HTSE OM</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Cap Market</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>FT CAPEX</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FT OM</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>CO2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>H2 PTC</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Electricity sales</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Naphta</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Diesel</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Jet fuel</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Storage CAPEX</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]Sheet1!$B$16:$M$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>-445702389.63329995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-324373084.37258297</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-182854574.46838459</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-198967386.2515654</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-232389965.06976801</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-663652627.02780199</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3059708327.5964799</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>147030.870178374</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>175167312.65753701</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>266844867.878654</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>487506058.74188602</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-5000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-90EA-8046-8EBE-135350765211}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]Sheet1!$A$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Davis-Besse</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$B$14:$M$14</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>HTSE CAPEX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>HTSE OM</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Cap Market</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>FT CAPEX</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FT OM</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>CO2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>H2 PTC</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Electricity sales</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Naphta</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Diesel</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Jet fuel</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Storage CAPEX</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]Sheet1!$B$17:$M$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>-528759325.05704498</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-390960462.95708597</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-212581225.27934557</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-226050666.882393</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-236403160.52235711</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-890215763.09717703</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3566914568.7290902</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>230544.65936366501</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>343875625.39085001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>323507771.63072997</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>607700986.01472199</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-5000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-90EA-8046-8EBE-135350765211}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]Sheet1!$A$18</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Prairie-Island</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$B$14:$M$14</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>HTSE CAPEX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>HTSE OM</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Cap Market</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>FT CAPEX</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FT OM</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>CO2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>H2 PTC</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Electricity sales</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Naphta</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Diesel</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Jet fuel</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Storage CAPEX</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]Sheet1!$B$18:$M$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>-308302047.21565998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-215306257.5244239</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-124114712.46592456</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-153929558.3589085</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-231368779.19221839</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-473249011.88508302</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2057406787.0966201</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4620752.2735904995</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>168074450.597473</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>172007346.60569799</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>296388471.49692601</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-17500000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-90EA-8046-8EBE-135350765211}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]Sheet1!$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>STP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$B$14:$M$14</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>HTSE CAPEX</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>HTSE OM</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Cap Market</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>FT CAPEX</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>FT OM</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>CO2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>H2 PTC</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Electricity sales</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Naphta</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Diesel</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Jet fuel</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Storage CAPEX</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]Sheet1!$B$19:$M$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>-735892434.635059</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-550901319.244735</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-304377122.98359358</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-283907522.79646802</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-236403160.52235711</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-2013144975.2023101</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5133263037.0468998</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>234983554.446565</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>300752335.53216898</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>522506051.25383598</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>915385484.95796096</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-200000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-90EA-8046-8EBE-135350765211}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="300"/>
-        <c:axId val="789935199"/>
-        <c:axId val="789936927"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="789935199"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="low"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="789936927"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="789936927"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>NPV</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                  <a:t> $bn (2020)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1400"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="789935199"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:dispUnits>
-          <c:builtInUnit val="billions"/>
-        </c:dispUnits>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -2571,7 +1773,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2622,7 +1824,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2654,7 +1856,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -2694,7 +1896,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -2750,35 +1952,6 @@
         <c:crossBetween val="between"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
-          <c:dispUnitsLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-          </c:dispUnitsLbl>
         </c:dispUnits>
       </c:valAx>
       <c:spPr>
@@ -2804,7 +1977,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2857,7 +2030,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3260,7 +2433,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3651,7 +2824,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4073,7 +3246,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4761,46 +3934,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -5307,7 +4440,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5511,6 +4644,509 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -5811,8 +5447,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6016,22 +5652,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6136,8 +5773,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6269,19 +5906,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6314,8 +5952,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6519,1016 +6157,6 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
@@ -7827,7 +6455,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8386,44 +7014,6 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2703CA3E-6460-F043-BAAE-1EC79A1CC02B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -8433,9 +7023,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1638300</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8454,7 +7044,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10245,7 +8835,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -10800,7 +9390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
   <dimension ref="A1:AK32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
@@ -11448,8 +10038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D846B4FC-CAF1-EA4A-9F31-BF425A354447}">
   <dimension ref="A1:Y48"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11555,43 +10145,43 @@
         <v>3408382538</v>
       </c>
       <c r="D2" s="3">
-        <v>-762820800.5</v>
+        <v>-762820801</v>
       </c>
       <c r="E2" s="3">
-        <v>-304078614.80000001</v>
+        <v>-304078615</v>
       </c>
       <c r="F2" s="3">
-        <v>-195937714.90000001</v>
+        <v>-195937715</v>
       </c>
       <c r="G2" s="3">
-        <v>-280143957.19999999</v>
+        <v>-280143957</v>
       </c>
       <c r="H2" s="3">
-        <v>347771988.80000001</v>
+        <v>347771989</v>
       </c>
       <c r="I2" s="3">
-        <v>-244831480.09999999</v>
+        <v>-244831480</v>
       </c>
       <c r="J2" s="3">
-        <v>-300272454.30000001</v>
+        <v>-300272454</v>
       </c>
       <c r="K2" s="3">
-        <v>-185018648.30000001</v>
+        <v>-185018648</v>
       </c>
       <c r="L2" s="3">
-        <v>-45790755.240000002</v>
+        <v>-45790755</v>
       </c>
       <c r="M2" s="3">
-        <v>-772932308.79999995</v>
+        <v>-772932309</v>
       </c>
       <c r="N2" s="3">
         <v>4780292061</v>
       </c>
       <c r="O2" s="3">
-        <v>136894993.59999999</v>
+        <v>136894994</v>
       </c>
       <c r="P2" s="3">
-        <v>-96374075.489999995</v>
+        <v>-96374075</v>
       </c>
       <c r="Q2" s="3">
         <v>-3543416.8</v>
@@ -11628,64 +10218,64 @@
       <c r="B3" s="3">
         <v>769</v>
       </c>
-      <c r="C3" s="3">
-        <v>1941429190</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="C3">
+        <v>1941429066.9816799</v>
+      </c>
+      <c r="D3">
         <v>-508716454.5</v>
       </c>
-      <c r="E3" s="3">
-        <v>-194630964</v>
-      </c>
-      <c r="F3" s="3">
-        <v>-129742120.40000001</v>
-      </c>
-      <c r="G3" s="3">
-        <v>-179311157.69999999</v>
-      </c>
-      <c r="H3" s="3">
-        <v>231925155.90000001</v>
-      </c>
-      <c r="I3" s="3">
-        <v>-168911091</v>
-      </c>
-      <c r="J3" s="3">
+      <c r="E3">
+        <v>-194630963.99524099</v>
+      </c>
+      <c r="F3">
+        <v>-129742120.369755</v>
+      </c>
+      <c r="G3">
+        <v>-179311157.69171801</v>
+      </c>
+      <c r="H3">
+        <v>231925155.90662</v>
+      </c>
+      <c r="I3">
+        <v>-168911091.03992</v>
+      </c>
+      <c r="J3">
         <v>-227097690.40000001</v>
       </c>
-      <c r="K3" s="3">
-        <v>-185018648.30000001</v>
-      </c>
-      <c r="L3" s="3">
-        <v>-47371316.810000002</v>
-      </c>
-      <c r="M3" s="3">
-        <v>-663652627</v>
-      </c>
-      <c r="N3" s="3">
-        <v>3059708328</v>
-      </c>
-      <c r="O3" s="3">
-        <v>103534428.2</v>
-      </c>
-      <c r="P3" s="3">
-        <v>-75404124.090000004</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>-3543416.8</v>
-      </c>
-      <c r="R3" s="3">
-        <v>147030.87</v>
-      </c>
-      <c r="S3" s="3">
-        <v>175167313</v>
-      </c>
-      <c r="T3" s="3">
-        <v>266844868</v>
-      </c>
-      <c r="U3" s="3">
-        <v>487506059</v>
-      </c>
-      <c r="V3" s="3">
+      <c r="K3">
+        <v>-185018648.255375</v>
+      </c>
+      <c r="L3">
+        <v>-47371316.814392999</v>
+      </c>
+      <c r="M3">
+        <v>-663652627.02780199</v>
+      </c>
+      <c r="N3">
+        <v>3059708327.5964799</v>
+      </c>
+      <c r="O3">
+        <v>103534428.236957</v>
+      </c>
+      <c r="P3">
+        <v>-75404124.088522404</v>
+      </c>
+      <c r="Q3">
+        <v>-3543416.77666657</v>
+      </c>
+      <c r="R3">
+        <v>146907.40594448999</v>
+      </c>
+      <c r="S3">
+        <v>175167312.65753701</v>
+      </c>
+      <c r="T3">
+        <v>266844867.878654</v>
+      </c>
+      <c r="U3">
+        <v>487506058.74188602</v>
+      </c>
+      <c r="V3">
         <v>-5000</v>
       </c>
       <c r="W3" s="11">
@@ -11705,65 +10295,65 @@
       <c r="B4" s="3">
         <v>894</v>
       </c>
-      <c r="C4" s="3">
-        <v>2357254371</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4">
+        <v>2357620907.3290401</v>
+      </c>
+      <c r="D4">
         <v>-584742286.5</v>
       </c>
-      <c r="E4" s="3">
-        <v>-226897370.5</v>
-      </c>
-      <c r="F4" s="3">
-        <v>-164063092.5</v>
-      </c>
-      <c r="G4" s="3">
-        <v>-209037808.5</v>
-      </c>
-      <c r="H4" s="3">
-        <v>266585530.69999999</v>
-      </c>
-      <c r="I4" s="3">
-        <v>-210602569.19999999</v>
-      </c>
-      <c r="J4" s="3">
+      <c r="E4">
+        <v>-226897370.493126</v>
+      </c>
+      <c r="F4">
+        <v>-163769794.49289399</v>
+      </c>
+      <c r="G4">
+        <v>-209037808.50267899</v>
+      </c>
+      <c r="H4">
+        <v>266585530.66260499</v>
+      </c>
+      <c r="I4">
+        <v>-210602569.21965</v>
+      </c>
+      <c r="J4">
         <v>-249984024</v>
       </c>
-      <c r="K4" s="3">
-        <v>-185018648.30000001</v>
-      </c>
-      <c r="L4" s="3">
-        <v>-51384512.270000003</v>
-      </c>
-      <c r="M4" s="3">
-        <v>-890215763.10000002</v>
-      </c>
-      <c r="N4" s="3">
-        <v>3566914569</v>
-      </c>
-      <c r="O4" s="3">
-        <v>113968367.3</v>
-      </c>
-      <c r="P4" s="3">
-        <v>-90035010.170000002</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>-3543416.8</v>
-      </c>
-      <c r="R4" s="3">
-        <v>230544.65900000001</v>
-      </c>
-      <c r="S4" s="3">
-        <v>343875625</v>
-      </c>
-      <c r="T4" s="3">
-        <v>323507772</v>
-      </c>
-      <c r="U4" s="3">
-        <v>607700986</v>
-      </c>
-      <c r="V4" s="3">
-        <v>-5000</v>
+      <c r="K4">
+        <v>-185018648.255375</v>
+      </c>
+      <c r="L4">
+        <v>-51384512.266982101</v>
+      </c>
+      <c r="M4">
+        <v>-890215763.09717703</v>
+      </c>
+      <c r="N4">
+        <v>3566914568.7290902</v>
+      </c>
+      <c r="O4">
+        <v>113968367.283283</v>
+      </c>
+      <c r="P4">
+        <v>-90035010.165675998</v>
+      </c>
+      <c r="Q4">
+        <v>-3543416.77666657</v>
+      </c>
+      <c r="R4">
+        <v>4820563.2221624199</v>
+      </c>
+      <c r="S4">
+        <v>343875625.39085001</v>
+      </c>
+      <c r="T4">
+        <v>323507771.63072997</v>
+      </c>
+      <c r="U4">
+        <v>607700986.01472199</v>
+      </c>
+      <c r="V4">
+        <v>-5000000</v>
       </c>
       <c r="W4" s="11">
         <v>3989837</v>
@@ -11782,65 +10372,65 @@
       <c r="B5" s="3">
         <v>522</v>
       </c>
-      <c r="C5" s="3">
-        <v>1177020404</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5">
+        <v>1186176051.1001599</v>
+      </c>
+      <c r="D5">
         <v>-354788741.69999999</v>
       </c>
-      <c r="E5" s="3">
-        <v>-130872544.8</v>
-      </c>
-      <c r="F5" s="3">
-        <v>-84433712.769999996</v>
-      </c>
-      <c r="G5" s="3">
-        <v>-120571295.7</v>
-      </c>
-      <c r="H5" s="3">
-        <v>161749110.90000001</v>
-      </c>
-      <c r="I5" s="3">
-        <v>-115262416.5</v>
-      </c>
-      <c r="J5" s="3">
+      <c r="E5">
+        <v>-130872544.755421</v>
+      </c>
+      <c r="F5">
+        <v>-85307645.409250796</v>
+      </c>
+      <c r="G5">
+        <v>-120571295.68925799</v>
+      </c>
+      <c r="H5">
+        <v>161749110.940222</v>
+      </c>
+      <c r="I5">
+        <v>-115262416.455882</v>
+      </c>
+      <c r="J5">
         <v>-177139512.40000001</v>
       </c>
-      <c r="K5" s="3">
-        <v>-185018648.30000001</v>
-      </c>
-      <c r="L5" s="3">
-        <v>-46350130.939999998</v>
-      </c>
-      <c r="M5" s="3">
-        <v>-473249011.89999998</v>
-      </c>
-      <c r="N5" s="3">
-        <v>2057406787</v>
-      </c>
-      <c r="O5" s="3">
-        <v>80758364.819999993</v>
-      </c>
-      <c r="P5" s="3">
-        <v>-57548410.780000001</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>-3543416.8</v>
-      </c>
-      <c r="R5" s="3">
-        <v>4620752.2699999996</v>
-      </c>
-      <c r="S5" s="3">
-        <v>168074451</v>
-      </c>
-      <c r="T5" s="3">
-        <v>172007347</v>
-      </c>
-      <c r="U5" s="3">
-        <v>296388471</v>
-      </c>
-      <c r="V5" s="3">
-        <v>-17500000</v>
+      <c r="K5">
+        <v>-185018648.255375</v>
+      </c>
+      <c r="L5">
+        <v>-46350130.936843403</v>
+      </c>
+      <c r="M5">
+        <v>-473249011.88508302</v>
+      </c>
+      <c r="N5">
+        <v>2057406787.0966201</v>
+      </c>
+      <c r="O5">
+        <v>80758364.823991895</v>
+      </c>
+      <c r="P5">
+        <v>-57548410.7829004</v>
+      </c>
+      <c r="Q5">
+        <v>-3543416.77666657</v>
+      </c>
+      <c r="R5">
+        <v>312267.29047446698</v>
+      </c>
+      <c r="S5">
+        <v>168074450.597473</v>
+      </c>
+      <c r="T5">
+        <v>172007346.60569799</v>
+      </c>
+      <c r="U5">
+        <v>296388471.49692601</v>
+      </c>
+      <c r="V5">
+        <v>-1000000</v>
       </c>
       <c r="W5" s="11">
         <v>3941392</v>
@@ -11859,65 +10449,65 @@
       <c r="B6" s="3">
         <v>1280</v>
       </c>
-      <c r="C6" s="3">
-        <v>2801411840</v>
-      </c>
-      <c r="D6" s="3">
-        <v>-813805836.5</v>
-      </c>
-      <c r="E6" s="3">
-        <v>-326536033.80000001</v>
-      </c>
-      <c r="F6" s="3">
-        <v>-224365285.5</v>
-      </c>
-      <c r="G6" s="3">
-        <v>-300833706.19999999</v>
-      </c>
-      <c r="H6" s="3">
-        <v>371016199.39999998</v>
-      </c>
-      <c r="I6" s="3">
-        <v>-293102797.60000002</v>
-      </c>
-      <c r="J6" s="3">
+      <c r="C6">
+        <v>3281939427.7312298</v>
+      </c>
+      <c r="D6">
+        <v>-81249856.590000004</v>
+      </c>
+      <c r="E6">
+        <v>-25813125.198307902</v>
+      </c>
+      <c r="F6">
+        <v>-1235478.77460742</v>
+      </c>
+      <c r="G6">
+        <v>-23781320.648768902</v>
+      </c>
+      <c r="H6">
+        <v>37042021.131117903</v>
+      </c>
+      <c r="I6">
+        <v>-29263196.6931425</v>
+      </c>
+      <c r="J6">
         <v>-313966536.69999999</v>
       </c>
-      <c r="K6" s="3">
-        <v>-185018648.30000001</v>
-      </c>
-      <c r="L6" s="3">
-        <v>-51384512.270000003</v>
-      </c>
-      <c r="M6" s="3">
-        <v>-2013144975</v>
-      </c>
-      <c r="N6" s="3">
-        <v>5133263037</v>
-      </c>
-      <c r="O6" s="3">
-        <v>143138161.40000001</v>
-      </c>
-      <c r="P6" s="3">
-        <v>-113079147.5</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>-3543416.8</v>
-      </c>
-      <c r="R6" s="3">
-        <v>234983554</v>
-      </c>
-      <c r="S6" s="3">
-        <v>300752336</v>
-      </c>
-      <c r="T6" s="3">
-        <v>522506051</v>
-      </c>
-      <c r="U6" s="3">
-        <v>915385485</v>
-      </c>
-      <c r="V6" s="3">
-        <v>-200000000</v>
+      <c r="K6">
+        <v>-185018648.255375</v>
+      </c>
+      <c r="L6">
+        <v>-51384512.266982101</v>
+      </c>
+      <c r="M6">
+        <v>-2013144975.2023101</v>
+      </c>
+      <c r="N6">
+        <v>5133263037.0468998</v>
+      </c>
+      <c r="O6">
+        <v>143138161.396833</v>
+      </c>
+      <c r="P6">
+        <v>-113079147.493301</v>
+      </c>
+      <c r="Q6">
+        <v>-3543416.77666657</v>
+      </c>
+      <c r="R6">
+        <v>2688374349.20362</v>
+      </c>
+      <c r="S6">
+        <v>300752335.53216898</v>
+      </c>
+      <c r="T6">
+        <v>522506051.25383598</v>
+      </c>
+      <c r="U6">
+        <v>915385484.95796096</v>
+      </c>
+      <c r="V6">
+        <v>-4000000000</v>
       </c>
       <c r="W6" s="11">
         <v>4010362</v>
@@ -13455,8 +12045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35F0C96-D3AA-4F4B-9456-DE375A306C8A}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V8" sqref="A8:V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add arma validation data to results
</commit_message>
<xml_diff>
--- a/use_cases/LWR_FT_2023/run/results.xlsx
+++ b/use_cases/LWR_FT_2023/run/results.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWR_FT_2023/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1443041-6972-864D-A147-4B2DE26A9F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDC1178-2F3B-DB42-8E60-FA7E13BB7AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17000" activeTab="2" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
+    <workbookView xWindow="40900" yWindow="3100" windowWidth="30720" windowHeight="17000" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="cases" sheetId="1" r:id="rId1"/>
-    <sheet name="cashflow_comparison" sheetId="5" r:id="rId2"/>
-    <sheet name="tallies" sheetId="7" r:id="rId3"/>
-    <sheet name="data" sheetId="4" r:id="rId4"/>
-    <sheet name="braidwood_SA" sheetId="2" r:id="rId5"/>
-    <sheet name="braidwood_h2ptc" sheetId="6" r:id="rId6"/>
+    <sheet name="arma validation" sheetId="8" r:id="rId1"/>
+    <sheet name="cases" sheetId="1" r:id="rId2"/>
+    <sheet name="cashflow_comparison" sheetId="5" r:id="rId3"/>
+    <sheet name="tallies" sheetId="7" r:id="rId4"/>
+    <sheet name="data" sheetId="4" r:id="rId5"/>
+    <sheet name="braidwood_SA" sheetId="2" r:id="rId6"/>
+    <sheet name="braidwood_h2ptc" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="183">
   <si>
     <t>Location</t>
   </si>
@@ -559,7 +560,37 @@
     <t>Yearly average production/consumption</t>
   </si>
   <si>
-    <t>=</t>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>kurtosis</t>
+  </si>
+  <si>
+    <t>skewness</t>
+  </si>
+  <si>
+    <t>Historical</t>
+  </si>
+  <si>
+    <t>Synthetic</t>
   </si>
 </sst>
 </file>
@@ -572,7 +603,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -601,6 +632,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -616,12 +660,119 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -630,7 +781,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -649,6 +800,30 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9113,6 +9288,406 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55707046-E177-6E43-A9F7-36F8F360A329}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="26"/>
+      <c r="B1" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="18"/>
+      <c r="F1" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="18"/>
+      <c r="J1" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="18"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="27"/>
+      <c r="B2" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="19">
+        <v>32.977089726027593</v>
+      </c>
+      <c r="C3" s="19">
+        <v>32.982069891257282</v>
+      </c>
+      <c r="D3" s="19">
+        <v>25.821181279965732</v>
+      </c>
+      <c r="E3" s="19">
+        <v>25.54626235988728</v>
+      </c>
+      <c r="F3" s="20">
+        <v>32.977089999999997</v>
+      </c>
+      <c r="G3" s="20">
+        <v>32.980620000000002</v>
+      </c>
+      <c r="H3" s="19">
+        <v>9.3756191019787352</v>
+      </c>
+      <c r="I3" s="19">
+        <v>9.375560755254849</v>
+      </c>
+      <c r="J3" s="20">
+        <v>41.194870000000002</v>
+      </c>
+      <c r="K3" s="21">
+        <v>41.570810000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="19">
+        <v>23.072473018716131</v>
+      </c>
+      <c r="C4" s="19">
+        <v>23.14013174622033</v>
+      </c>
+      <c r="D4" s="19">
+        <v>110.32042329668749</v>
+      </c>
+      <c r="E4" s="19">
+        <v>110.57936084123359</v>
+      </c>
+      <c r="F4" s="20">
+        <v>23.072469999999999</v>
+      </c>
+      <c r="G4" s="20">
+        <v>23.11992</v>
+      </c>
+      <c r="H4" s="19">
+        <v>15.093720414581179</v>
+      </c>
+      <c r="I4" s="19">
+        <v>15.06729275093023</v>
+      </c>
+      <c r="J4" s="20">
+        <v>290.6533</v>
+      </c>
+      <c r="K4" s="21">
+        <v>290.52300000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" s="19">
+        <v>2.27</v>
+      </c>
+      <c r="C5" s="19">
+        <v>2.27</v>
+      </c>
+      <c r="D5" s="19">
+        <v>-65.109300000000005</v>
+      </c>
+      <c r="E5" s="19">
+        <v>-65.109300000000005</v>
+      </c>
+      <c r="F5" s="20">
+        <v>2.27</v>
+      </c>
+      <c r="G5" s="20">
+        <v>2.27</v>
+      </c>
+      <c r="H5" s="19">
+        <v>-66.2</v>
+      </c>
+      <c r="I5" s="19">
+        <v>-66.2</v>
+      </c>
+      <c r="J5" s="20">
+        <v>-20.2</v>
+      </c>
+      <c r="K5" s="21">
+        <v>-20.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="19">
+        <v>22.72</v>
+      </c>
+      <c r="C6" s="19">
+        <v>22.643500327024999</v>
+      </c>
+      <c r="D6" s="19">
+        <v>14.7645</v>
+      </c>
+      <c r="E6" s="19">
+        <v>14.37777231055</v>
+      </c>
+      <c r="F6" s="20">
+        <v>22.72</v>
+      </c>
+      <c r="G6" s="20">
+        <v>22.64517</v>
+      </c>
+      <c r="H6" s="19">
+        <v>-0.48</v>
+      </c>
+      <c r="I6" s="19">
+        <v>-0.57533928877825002</v>
+      </c>
+      <c r="J6" s="20">
+        <v>18.850000000000001</v>
+      </c>
+      <c r="K6" s="21">
+        <v>16.82328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="19">
+        <v>28.84</v>
+      </c>
+      <c r="C7" s="19">
+        <v>28.838039755650001</v>
+      </c>
+      <c r="D7" s="19">
+        <v>19.299150000000001</v>
+      </c>
+      <c r="E7" s="19">
+        <v>19.173366480049999</v>
+      </c>
+      <c r="F7" s="20">
+        <v>28.84</v>
+      </c>
+      <c r="G7" s="20">
+        <v>28.829719999999998</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0.46</v>
+      </c>
+      <c r="I7" s="19">
+        <v>0.58024959424</v>
+      </c>
+      <c r="J7" s="20">
+        <v>23.93</v>
+      </c>
+      <c r="K7" s="21">
+        <v>24.394089999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="19">
+        <v>37</v>
+      </c>
+      <c r="C8" s="19">
+        <v>37.050237273224987</v>
+      </c>
+      <c r="D8" s="19">
+        <v>27.236725</v>
+      </c>
+      <c r="E8" s="19">
+        <v>27.222851138425</v>
+      </c>
+      <c r="F8" s="20">
+        <v>37</v>
+      </c>
+      <c r="G8" s="20">
+        <v>37.050960000000003</v>
+      </c>
+      <c r="H8" s="19">
+        <v>21.48</v>
+      </c>
+      <c r="I8" s="19">
+        <v>21.463601906800001</v>
+      </c>
+      <c r="J8" s="20">
+        <v>32.020000000000003</v>
+      </c>
+      <c r="K8" s="21">
+        <v>36.356409999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="19">
+        <v>933.68</v>
+      </c>
+      <c r="C9" s="19">
+        <v>933.68</v>
+      </c>
+      <c r="D9" s="19">
+        <v>4230.9575999999997</v>
+      </c>
+      <c r="E9" s="19">
+        <v>4230.9575999999997</v>
+      </c>
+      <c r="F9" s="20">
+        <v>933.68</v>
+      </c>
+      <c r="G9" s="20">
+        <v>933.68</v>
+      </c>
+      <c r="H9" s="19">
+        <v>97</v>
+      </c>
+      <c r="I9" s="19">
+        <v>97</v>
+      </c>
+      <c r="J9" s="20">
+        <v>8996.83</v>
+      </c>
+      <c r="K9" s="21">
+        <v>8996.83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="19">
+        <v>243.2975401419815</v>
+      </c>
+      <c r="C10" s="19">
+        <v>241.7648380101034</v>
+      </c>
+      <c r="D10" s="19">
+        <v>755.89628240068259</v>
+      </c>
+      <c r="E10" s="19">
+        <v>749.96335094363985</v>
+      </c>
+      <c r="F10" s="20">
+        <v>243.29750000000001</v>
+      </c>
+      <c r="G10" s="20">
+        <v>241.2045</v>
+      </c>
+      <c r="H10" s="19">
+        <v>1.2113442580170011</v>
+      </c>
+      <c r="I10" s="19">
+        <v>1.2223387323406909</v>
+      </c>
+      <c r="J10" s="20">
+        <v>699.61369999999999</v>
+      </c>
+      <c r="K10" s="21">
+        <v>696.71950000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" s="22">
+        <v>10.85681406844434</v>
+      </c>
+      <c r="C11" s="22">
+        <v>10.81196311074452</v>
+      </c>
+      <c r="D11" s="22">
+        <v>26.76559217679149</v>
+      </c>
+      <c r="E11" s="22">
+        <v>26.607204309125571</v>
+      </c>
+      <c r="F11" s="23">
+        <v>10.856809999999999</v>
+      </c>
+      <c r="G11" s="23">
+        <v>10.79345</v>
+      </c>
+      <c r="H11" s="22">
+        <v>1.292473562594213</v>
+      </c>
+      <c r="I11" s="22">
+        <v>1.297771260495596</v>
+      </c>
+      <c r="J11" s="23">
+        <v>25.769310000000001</v>
+      </c>
+      <c r="K11" s="24">
+        <v>25.698989999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
   <dimension ref="A1:AK32"/>
   <sheetViews>
@@ -9760,7 +10335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D846B4FC-CAF1-EA4A-9F31-BF425A354447}">
   <dimension ref="A1:Y48"/>
   <sheetViews>
@@ -11767,11 +12342,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB61019-C971-8A49-90D4-C01E93F6857E}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -12201,9 +12776,6 @@
       <c r="A20" t="s">
         <v>133</v>
       </c>
-      <c r="B20" t="s">
-        <v>172</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -12220,7 +12792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35F0C96-D3AA-4F4B-9456-DE375A306C8A}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
@@ -12787,7 +13359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA1661-1357-8E4D-8878-EEFCBAD9628D}">
   <dimension ref="A1:N23"/>
   <sheetViews>
@@ -13444,7 +14016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAC29D9-F38F-D947-8D8F-5B3E6EFFC85F}">
   <dimension ref="A1:F13"/>
   <sheetViews>

</xml_diff>